<commit_message>
Add data mapping functionality and Excel file handling
</commit_message>
<xml_diff>
--- a/mapped_output.xlsx
+++ b/mapped_output.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amedeloitte-my.sharepoint.com/personal/kchhatbar_deloitte_com/Documents/Documents/AMEX/copilot/data_mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2B59D2BFD3B05B4313BA3B1159CC28F34B83E056" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BF40BBD-356F-4D7E-86D4-7338C5D2E461}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_748733BB4A70D307353F61C05CB4BC191391903D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8FA2F65-6DBD-4CC4-A7A5-1A0C64B9800E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="94">
   <si>
     <t>FIRST_NAME</t>
   </si>
@@ -260,6 +273,48 @@
   </si>
   <si>
     <t>sophie.c</t>
+  </si>
+  <si>
+    <t>Emp_Id</t>
+  </si>
+  <si>
+    <t>FULL_NAME</t>
+  </si>
+  <si>
+    <t>JOHN Doe</t>
+  </si>
+  <si>
+    <t>JANE Smith</t>
+  </si>
+  <si>
+    <t>ROBERT Johnson</t>
+  </si>
+  <si>
+    <t>MARIA Garcia</t>
+  </si>
+  <si>
+    <t>DAVID Brown</t>
+  </si>
+  <si>
+    <t>SARAH Wilson</t>
+  </si>
+  <si>
+    <t>MICHAEL Taylor</t>
+  </si>
+  <si>
+    <t>EMMA Anderson</t>
+  </si>
+  <si>
+    <t>JAMES Martinez</t>
+  </si>
+  <si>
+    <t>LISA Thompson</t>
+  </si>
+  <si>
+    <t>WILLIAM White</t>
+  </si>
+  <si>
+    <t>SOPHIE Clark</t>
   </si>
 </sst>
 </file>
@@ -622,363 +677,443 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>21</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>45</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>26</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>27</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>30</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>31</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>32</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>20</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>33</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>36</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>35</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>37</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>38</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>13</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>39</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
         <v>41</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>42</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>42</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>43</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>44</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>13</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>45</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" t="s">
         <v>47</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>48</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>33</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>49</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>50</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>13</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>51</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" t="s">
         <v>52</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>53</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>29</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>54</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>55</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>20</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>56</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
         <v>58</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>59</v>
       </c>
-      <c r="C10">
+      <c r="E10">
         <v>38</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>60</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>61</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" t="s">
         <v>13</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>62</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
         <v>63</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>64</v>
       </c>
-      <c r="C11">
+      <c r="E11">
         <v>31</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>65</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>66</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
         <v>13</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J11" t="s">
         <v>67</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" t="s">
         <v>69</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>70</v>
       </c>
-      <c r="C12">
+      <c r="E12">
         <v>47</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>71</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>72</v>
       </c>
-      <c r="G12" t="s">
+      <c r="I12" t="s">
         <v>26</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J12" t="s">
         <v>73</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" t="s">
         <v>75</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>76</v>
       </c>
-      <c r="C13">
+      <c r="E13">
         <v>26</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
         <v>77</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>78</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
         <v>20</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J13" t="s">
         <v>79</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K13" t="s">
         <v>46</v>
       </c>
     </row>
@@ -989,6 +1124,6 @@
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{ea60d57e-af5b-4752-ac57-3e4f28ca11dc}" enabled="1" method="Standard" siteId="{36da45f1-dd2c-4d1f-af13-5abe46b99921}" removed="0"/>
+  <clbl:label id="{ea60d57e-af5b-4752-ac57-3e4f28ca11dc}" enabled="1" method="Standard" siteId="{36da45f1-dd2c-4d1f-af13-5abe46b99921}" contentBits="0" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>